<commit_message>
add hasMany option for joinables
</commit_message>
<xml_diff>
--- a/tests/Feature/JoinBelongsToNestedTest/joinable_dummies.xlsx
+++ b/tests/Feature/JoinBelongsToNestedTest/joinable_dummies.xlsx
@@ -31,16 +31,16 @@
     <t xml:space="preserve">description</t>
   </si>
   <si>
-    <t xml:space="preserve">joinable_relations.id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">joinable_relations.foreign_field</t>
-  </si>
-  <si>
-    <t xml:space="preserve">joinable_relations.another_foreign_field</t>
-  </si>
-  <si>
-    <t xml:space="preserve">joinable_relations.nested_joinable_relations.foreign_field</t>
+    <t xml:space="preserve">joinable_relation.id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">joinable_relation.foreign_field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">joinable_relation.another_foreign_field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">joinable_relation.nested_joinable_relation.foreign_field</t>
   </si>
   <si>
     <t xml:space="preserve">title 1</t>

</xml_diff>